<commit_message>
Adding notes to template
</commit_message>
<xml_diff>
--- a/schema_definitions/study_schema.xlsx
+++ b/schema_definitions/study_schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC4558-9E5E-2E4A-BDA2-40D5506879A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89610B38-E240-EC47-9887-D703BEEF5505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51620" yWindow="-4160" windowWidth="28360" windowHeight="24540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>The method used to genotype variants in the discovery stage</t>
   </si>
   <si>
-    <t>Genome-wide genotyping array</t>
-  </si>
-  <si>
     <t>Genome-wide genotyping array|Targeted genotyping array|Exome genotyping array|Whole genome sequencing</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>The trait under investigation</t>
+  </si>
+  <si>
+    <t>Targeted genotyping array</t>
   </si>
 </sst>
 </file>
@@ -618,16 +618,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="96" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -679,10 +681,10 @@
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -699,16 +701,16 @@
         <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -716,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -725,10 +727,10 @@
         <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -736,7 +738,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -745,10 +747,10 @@
         <v>25</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -756,25 +758,25 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>51</v>
-      </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -782,19 +784,19 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -802,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -811,10 +813,10 @@
         <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -822,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -831,10 +833,10 @@
         <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -842,7 +844,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -851,13 +853,13 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -865,7 +867,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -874,13 +876,13 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -888,7 +890,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -897,13 +899,13 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -911,7 +913,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -920,13 +922,13 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -934,7 +936,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -943,18 +945,18 @@
         <v>25</v>
       </c>
       <c r="I14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -963,13 +965,13 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
         <v>62</v>
       </c>
-      <c r="I15" t="s">
-        <v>63</v>
-      </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding summary stats checksum to study table
</commit_message>
<xml_diff>
--- a/schema_definitions/study_schema.xlsx
+++ b/schema_definitions/study_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C6E19D-2E12-8C40-A1D4-6AE29C81BDD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1A6F07-C5BA-9540-9B6F-A300659F579C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="35440" yWindow="-1520" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>NAME</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>cheksum</t>
+  </si>
+  <si>
+    <t>md5 checksum of the summary stats file</t>
+  </si>
+  <si>
+    <t>md5 sum</t>
   </si>
 </sst>
 </file>
@@ -619,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,27 +1008,47 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
         <v>61</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" t="s">
         <v>62</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L16" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>